<commit_message>
Update MS-ASRM RS file
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASRM/MS-ASRM_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASRM/MS-ASRM_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4145EABB-8E85-46BC-8013-805E66049144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743452C1-248E-42C1-88A7-CEFF2AB65961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -1840,9 +1840,6 @@
     <t>[In RightsManagementSupport] If the value of this element[RightsManagementSupport] is TRUE (1), the server will decompress rights-managed email messages before sending them to the client, as specified in section 3.2.4.3.</t>
   </si>
   <si>
-    <t>[In RightsManagementSupport] If the value of this element[RightsManagementSupport] is TRUE (1), the server will decrypt rights-managed email messages before sending them to the client, as specified in section 3.2.4.3.</t>
-  </si>
-  <si>
     <t>[In RightsManagementSupport] If the value is FALSE (0), the server will not decompress rights-managed email messages before sending them to the client.</t>
   </si>
   <si>
@@ -3435,6 +3432,9 @@
   </si>
   <si>
     <t>10.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[In RightsManagementSupport] If the value of this element[RightsManagementSupport] is TRUE (1), the server will decompress and decrypt rights-managed email messages before sending them to the client, as specified in section 3.2.4.3. </t>
   </si>
 </sst>
 </file>
@@ -3733,21 +3733,6 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3771,6 +3756,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6101,8 +6101,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L497"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:I8"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C233" sqref="C233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -6122,7 +6122,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -6132,7 +6132,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -6146,10 +6146,10 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F3" s="12">
         <v>43374</v>
@@ -6157,127 +6157,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -6290,12 +6290,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -6308,12 +6308,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -6326,12 +6326,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -6344,60 +6344,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -6464,7 +6464,7 @@
         <v>388</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22" t="s">
@@ -6689,7 +6689,7 @@
         <v>391</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -6739,7 +6739,7 @@
         <v>391</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22" t="s">
@@ -6814,7 +6814,7 @@
         <v>391</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29" t="s">
@@ -6839,7 +6839,7 @@
         <v>391</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29" t="s">
@@ -6864,7 +6864,7 @@
         <v>391</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29" t="s">
@@ -7014,7 +7014,7 @@
         <v>392</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29" t="s">
@@ -7108,13 +7108,13 @@
     </row>
     <row r="47" spans="1:9" ht="30">
       <c r="A47" s="22" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B47" s="30" t="s">
         <v>392</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="22" t="s">
@@ -7133,13 +7133,13 @@
     </row>
     <row r="48" spans="1:9" ht="30">
       <c r="A48" s="22" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B48" s="30" t="s">
         <v>392</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22" t="s">
@@ -7158,13 +7158,13 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="22" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B49" s="30" t="s">
         <v>392</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="22" t="s">
@@ -7183,13 +7183,13 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="22" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B50" s="30" t="s">
         <v>392</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="22" t="s">
@@ -7208,13 +7208,13 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="22" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B51" s="30" t="s">
         <v>392</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D51" s="36"/>
       <c r="E51" s="22" t="s">
@@ -7314,7 +7314,7 @@
         <v>393</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29" t="s">
@@ -7333,13 +7333,13 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="22" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B56" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D56" s="36"/>
       <c r="E56" s="29" t="s">
@@ -7405,7 +7405,7 @@
         <v>17</v>
       </c>
       <c r="I58" s="31" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -7419,7 +7419,7 @@
         <v>457</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E59" s="29" t="s">
         <v>19</v>
@@ -7437,13 +7437,13 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="22" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B60" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D60" s="22"/>
       <c r="E60" s="22" t="s">
@@ -7462,13 +7462,13 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="22" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B61" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D61" s="22"/>
       <c r="E61" s="22" t="s">
@@ -7487,13 +7487,13 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="22" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B62" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D62" s="22"/>
       <c r="E62" s="22" t="s">
@@ -7512,13 +7512,13 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="22" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B63" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D63" s="22"/>
       <c r="E63" s="22" t="s">
@@ -7537,13 +7537,13 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="22" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B64" s="30" t="s">
         <v>393</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D64" s="36"/>
       <c r="E64" s="22" t="s">
@@ -7643,7 +7643,7 @@
         <v>394</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -7662,13 +7662,13 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="22" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B69" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29" t="s">
@@ -7687,13 +7687,13 @@
     </row>
     <row r="70" spans="1:9" ht="30">
       <c r="A70" s="22" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B70" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="29" t="s">
@@ -7718,7 +7718,7 @@
         <v>394</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D71" s="29"/>
       <c r="E71" s="29" t="s">
@@ -7768,7 +7768,7 @@
         <v>394</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29" t="s">
@@ -7793,7 +7793,7 @@
         <v>394</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D74" s="29"/>
       <c r="E74" s="29" t="s">
@@ -7843,7 +7843,7 @@
         <v>394</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D76" s="29"/>
       <c r="E76" s="29" t="s">
@@ -7887,13 +7887,13 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="22" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B78" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D78" s="22"/>
       <c r="E78" s="22" t="s">
@@ -7912,13 +7912,13 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="22" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B79" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D79" s="22"/>
       <c r="E79" s="22" t="s">
@@ -7937,13 +7937,13 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="22" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B80" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D80" s="22"/>
       <c r="E80" s="22" t="s">
@@ -7962,13 +7962,13 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="22" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B81" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D81" s="22"/>
       <c r="E81" s="22" t="s">
@@ -7987,13 +7987,13 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="22" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B82" s="30" t="s">
         <v>394</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D82" s="22"/>
       <c r="E82" s="22" t="s">
@@ -8093,7 +8093,7 @@
         <v>395</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D86" s="29"/>
       <c r="E86" s="29" t="s">
@@ -8118,7 +8118,7 @@
         <v>395</v>
       </c>
       <c r="C87" s="20" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D87" s="29"/>
       <c r="E87" s="29" t="s">
@@ -8143,7 +8143,7 @@
         <v>395</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D88" s="29"/>
       <c r="E88" s="29" t="s">
@@ -8168,7 +8168,7 @@
         <v>395</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D89" s="29"/>
       <c r="E89" s="29" t="s">
@@ -8193,7 +8193,7 @@
         <v>395</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D90" s="29"/>
       <c r="E90" s="29" t="s">
@@ -8218,7 +8218,7 @@
         <v>395</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D91" s="29"/>
       <c r="E91" s="29" t="s">
@@ -8243,7 +8243,7 @@
         <v>395</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D92" s="29"/>
       <c r="E92" s="29" t="s">
@@ -8337,13 +8337,13 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="22" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B96" s="30" t="s">
         <v>395</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D96" s="22"/>
       <c r="E96" s="22" t="s">
@@ -8362,13 +8362,13 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="22" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B97" s="30" t="s">
         <v>395</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D97" s="22"/>
       <c r="E97" s="22" t="s">
@@ -8387,13 +8387,13 @@
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="22" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B98" s="30" t="s">
         <v>395</v>
       </c>
       <c r="C98" s="20" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D98" s="22"/>
       <c r="E98" s="22" t="s">
@@ -8412,13 +8412,13 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="22" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B99" s="30" t="s">
         <v>395</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D99" s="22"/>
       <c r="E99" s="22" t="s">
@@ -8437,13 +8437,13 @@
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="22" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B100" s="30" t="s">
         <v>395</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D100" s="22"/>
       <c r="E100" s="22" t="s">
@@ -8543,7 +8543,7 @@
         <v>396</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D104" s="29"/>
       <c r="E104" s="29" t="s">
@@ -8568,7 +8568,7 @@
         <v>396</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D105" s="29"/>
       <c r="E105" s="29" t="s">
@@ -8612,13 +8612,13 @@
     </row>
     <row r="107" spans="1:9">
       <c r="A107" s="22" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B107" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C107" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D107" s="22"/>
       <c r="E107" s="22" t="s">
@@ -8637,13 +8637,13 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="22" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B108" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D108" s="22"/>
       <c r="E108" s="22" t="s">
@@ -8662,13 +8662,13 @@
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="22" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B109" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D109" s="22"/>
       <c r="E109" s="22" t="s">
@@ -8687,13 +8687,13 @@
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="22" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B110" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C110" s="20" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D110" s="22"/>
       <c r="E110" s="22" t="s">
@@ -8712,13 +8712,13 @@
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="22" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B111" s="30" t="s">
         <v>396</v>
       </c>
       <c r="C111" s="20" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D111" s="22"/>
       <c r="E111" s="22" t="s">
@@ -8818,7 +8818,7 @@
         <v>397</v>
       </c>
       <c r="C115" s="20" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29" t="s">
@@ -8843,7 +8843,7 @@
         <v>397</v>
       </c>
       <c r="C116" s="20" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="29" t="s">
@@ -8887,13 +8887,13 @@
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="22" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B118" s="30" t="s">
         <v>397</v>
       </c>
       <c r="C118" s="20" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D118" s="22"/>
       <c r="E118" s="22" t="s">
@@ -8912,13 +8912,13 @@
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="22" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B119" s="30" t="s">
         <v>397</v>
       </c>
       <c r="C119" s="20" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D119" s="22"/>
       <c r="E119" s="22" t="s">
@@ -8937,13 +8937,13 @@
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="22" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B120" s="30" t="s">
         <v>397</v>
       </c>
       <c r="C120" s="20" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D120" s="22"/>
       <c r="E120" s="22" t="s">
@@ -8962,13 +8962,13 @@
     </row>
     <row r="121" spans="1:9">
       <c r="A121" s="22" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B121" s="30" t="s">
         <v>397</v>
       </c>
       <c r="C121" s="20" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D121" s="22"/>
       <c r="E121" s="22" t="s">
@@ -8987,13 +8987,13 @@
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="22" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B122" s="30" t="s">
         <v>397</v>
       </c>
       <c r="C122" s="20" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D122" s="22"/>
       <c r="E122" s="22" t="s">
@@ -9043,7 +9043,7 @@
         <v>398</v>
       </c>
       <c r="C124" s="20" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D124" s="29"/>
       <c r="E124" s="29" t="s">
@@ -9093,7 +9093,7 @@
         <v>398</v>
       </c>
       <c r="C126" s="20" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="29" t="s">
@@ -9118,7 +9118,7 @@
         <v>398</v>
       </c>
       <c r="C127" s="20" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="29" t="s">
@@ -9137,13 +9137,13 @@
     </row>
     <row r="128" spans="1:9" ht="30">
       <c r="A128" s="22" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B128" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="22" t="s">
@@ -9187,13 +9187,13 @@
     </row>
     <row r="130" spans="1:9" ht="30">
       <c r="A130" s="22" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B130" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C130" s="20" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D130" s="22"/>
       <c r="E130" s="22" t="s">
@@ -9212,13 +9212,13 @@
     </row>
     <row r="131" spans="1:9" ht="30">
       <c r="A131" s="22" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B131" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D131" s="22"/>
       <c r="E131" s="22" t="s">
@@ -9237,13 +9237,13 @@
     </row>
     <row r="132" spans="1:9" ht="30">
       <c r="A132" s="22" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B132" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C132" s="20" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D132" s="22"/>
       <c r="E132" s="22" t="s">
@@ -9262,13 +9262,13 @@
     </row>
     <row r="133" spans="1:9" ht="30">
       <c r="A133" s="22" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B133" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C133" s="20" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D133" s="22"/>
       <c r="E133" s="22" t="s">
@@ -9287,13 +9287,13 @@
     </row>
     <row r="134" spans="1:9" ht="30">
       <c r="A134" s="22" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B134" s="30" t="s">
         <v>398</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="D134" s="36"/>
       <c r="E134" s="22" t="s">
@@ -9393,7 +9393,7 @@
         <v>399</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="29" t="s">
@@ -9418,7 +9418,7 @@
         <v>399</v>
       </c>
       <c r="C139" s="20" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="29" t="s">
@@ -9537,13 +9537,13 @@
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="22" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B144" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C144" s="20" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D144" s="22"/>
       <c r="E144" s="22" t="s">
@@ -9562,13 +9562,13 @@
     </row>
     <row r="145" spans="1:9">
       <c r="A145" s="22" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B145" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C145" s="20" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D145" s="22"/>
       <c r="E145" s="22" t="s">
@@ -9587,13 +9587,13 @@
     </row>
     <row r="146" spans="1:9">
       <c r="A146" s="22" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B146" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C146" s="20" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D146" s="22"/>
       <c r="E146" s="22" t="s">
@@ -9612,13 +9612,13 @@
     </row>
     <row r="147" spans="1:9">
       <c r="A147" s="22" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B147" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C147" s="20" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D147" s="22"/>
       <c r="E147" s="22" t="s">
@@ -9637,13 +9637,13 @@
     </row>
     <row r="148" spans="1:9">
       <c r="A148" s="22" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B148" s="30" t="s">
         <v>399</v>
       </c>
       <c r="C148" s="20" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="D148" s="36"/>
       <c r="E148" s="22" t="s">
@@ -9768,7 +9768,7 @@
         <v>400</v>
       </c>
       <c r="C153" s="20" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="29" t="s">
@@ -9793,7 +9793,7 @@
         <v>400</v>
       </c>
       <c r="C154" s="20" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="29" t="s">
@@ -9837,13 +9837,13 @@
     </row>
     <row r="156" spans="1:9">
       <c r="A156" s="22" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B156" s="30" t="s">
         <v>400</v>
       </c>
       <c r="C156" s="20" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D156" s="22"/>
       <c r="E156" s="22" t="s">
@@ -9862,13 +9862,13 @@
     </row>
     <row r="157" spans="1:9">
       <c r="A157" s="22" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B157" s="30" t="s">
         <v>400</v>
       </c>
       <c r="C157" s="20" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D157" s="22"/>
       <c r="E157" s="22" t="s">
@@ -9887,13 +9887,13 @@
     </row>
     <row r="158" spans="1:9">
       <c r="A158" s="22" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B158" s="30" t="s">
         <v>400</v>
       </c>
       <c r="C158" s="20" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D158" s="22"/>
       <c r="E158" s="22" t="s">
@@ -9912,13 +9912,13 @@
     </row>
     <row r="159" spans="1:9">
       <c r="A159" s="22" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B159" s="30" t="s">
         <v>400</v>
       </c>
       <c r="C159" s="20" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D159" s="22"/>
       <c r="E159" s="22" t="s">
@@ -9937,13 +9937,13 @@
     </row>
     <row r="160" spans="1:9">
       <c r="A160" s="22" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B160" s="30" t="s">
         <v>400</v>
       </c>
       <c r="C160" s="20" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D160" s="36"/>
       <c r="E160" s="22" t="s">
@@ -10043,7 +10043,7 @@
         <v>401</v>
       </c>
       <c r="C164" s="20" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D164" s="29"/>
       <c r="E164" s="29" t="s">
@@ -10068,7 +10068,7 @@
         <v>401</v>
       </c>
       <c r="C165" s="20" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="29" t="s">
@@ -10137,13 +10137,13 @@
     </row>
     <row r="168" spans="1:9" ht="30">
       <c r="A168" s="22" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B168" s="30" t="s">
         <v>401</v>
       </c>
       <c r="C168" s="20" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D168" s="22"/>
       <c r="E168" s="22" t="s">
@@ -10162,13 +10162,13 @@
     </row>
     <row r="169" spans="1:9" ht="30">
       <c r="A169" s="22" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B169" s="30" t="s">
         <v>401</v>
       </c>
       <c r="C169" s="20" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D169" s="22"/>
       <c r="E169" s="22" t="s">
@@ -10187,13 +10187,13 @@
     </row>
     <row r="170" spans="1:9" ht="30">
       <c r="A170" s="22" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B170" s="30" t="s">
         <v>401</v>
       </c>
       <c r="C170" s="20" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D170" s="22"/>
       <c r="E170" s="22" t="s">
@@ -10212,13 +10212,13 @@
     </row>
     <row r="171" spans="1:9" ht="30">
       <c r="A171" s="22" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B171" s="30" t="s">
         <v>401</v>
       </c>
       <c r="C171" s="20" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D171" s="22"/>
       <c r="E171" s="22" t="s">
@@ -10237,13 +10237,13 @@
     </row>
     <row r="172" spans="1:9" ht="30">
       <c r="A172" s="22" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B172" s="30" t="s">
         <v>401</v>
       </c>
       <c r="C172" s="20" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D172" s="36"/>
       <c r="E172" s="22" t="s">
@@ -10268,7 +10268,7 @@
         <v>402</v>
       </c>
       <c r="C173" s="20" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="D173" s="29"/>
       <c r="E173" s="29" t="s">
@@ -10387,13 +10387,13 @@
     </row>
     <row r="178" spans="1:9" ht="30">
       <c r="A178" s="22" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B178" s="30" t="s">
         <v>402</v>
       </c>
       <c r="C178" s="20" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D178" s="22"/>
       <c r="E178" s="22" t="s">
@@ -10412,13 +10412,13 @@
     </row>
     <row r="179" spans="1:9" ht="30">
       <c r="A179" s="22" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B179" s="30" t="s">
         <v>402</v>
       </c>
       <c r="C179" s="20" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D179" s="22"/>
       <c r="E179" s="22" t="s">
@@ -10437,13 +10437,13 @@
     </row>
     <row r="180" spans="1:9" ht="30">
       <c r="A180" s="22" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B180" s="30" t="s">
         <v>402</v>
       </c>
       <c r="C180" s="20" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D180" s="22"/>
       <c r="E180" s="22" t="s">
@@ -10462,13 +10462,13 @@
     </row>
     <row r="181" spans="1:9" ht="30">
       <c r="A181" s="22" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B181" s="30" t="s">
         <v>402</v>
       </c>
       <c r="C181" s="20" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D181" s="22"/>
       <c r="E181" s="22" t="s">
@@ -10487,13 +10487,13 @@
     </row>
     <row r="182" spans="1:9" ht="30">
       <c r="A182" s="22" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B182" s="30" t="s">
         <v>402</v>
       </c>
       <c r="C182" s="20" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D182" s="36"/>
       <c r="E182" s="22" t="s">
@@ -10543,7 +10543,7 @@
         <v>403</v>
       </c>
       <c r="C184" s="20" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="29" t="s">
@@ -10593,7 +10593,7 @@
         <v>403</v>
       </c>
       <c r="C186" s="20" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D186" s="29"/>
       <c r="E186" s="29" t="s">
@@ -10618,7 +10618,7 @@
         <v>403</v>
       </c>
       <c r="C187" s="20" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D187" s="29"/>
       <c r="E187" s="29" t="s">
@@ -10662,13 +10662,13 @@
     </row>
     <row r="189" spans="1:9" ht="30">
       <c r="A189" s="22" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B189" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C189" s="20" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D189" s="22"/>
       <c r="E189" s="22" t="s">
@@ -10687,13 +10687,13 @@
     </row>
     <row r="190" spans="1:9" ht="30">
       <c r="A190" s="22" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B190" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C190" s="20" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D190" s="22"/>
       <c r="E190" s="22" t="s">
@@ -10712,13 +10712,13 @@
     </row>
     <row r="191" spans="1:9">
       <c r="A191" s="22" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B191" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C191" s="20" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D191" s="22"/>
       <c r="E191" s="22" t="s">
@@ -10737,13 +10737,13 @@
     </row>
     <row r="192" spans="1:9">
       <c r="A192" s="22" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B192" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C192" s="20" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D192" s="22"/>
       <c r="E192" s="22" t="s">
@@ -10762,13 +10762,13 @@
     </row>
     <row r="193" spans="1:9">
       <c r="A193" s="22" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B193" s="30" t="s">
         <v>403</v>
       </c>
       <c r="C193" s="20" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="D193" s="36"/>
       <c r="E193" s="22" t="s">
@@ -10868,7 +10868,7 @@
         <v>404</v>
       </c>
       <c r="C197" s="20" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D197" s="29"/>
       <c r="E197" s="29" t="s">
@@ -10893,7 +10893,7 @@
         <v>404</v>
       </c>
       <c r="C198" s="20" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="29" t="s">
@@ -10937,13 +10937,13 @@
     </row>
     <row r="200" spans="1:9">
       <c r="A200" s="22" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B200" s="30" t="s">
         <v>404</v>
       </c>
       <c r="C200" s="20" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D200" s="22"/>
       <c r="E200" s="22" t="s">
@@ -10962,13 +10962,13 @@
     </row>
     <row r="201" spans="1:9">
       <c r="A201" s="22" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B201" s="30" t="s">
         <v>404</v>
       </c>
       <c r="C201" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D201" s="22"/>
       <c r="E201" s="22" t="s">
@@ -10987,13 +10987,13 @@
     </row>
     <row r="202" spans="1:9">
       <c r="A202" s="22" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B202" s="30" t="s">
         <v>404</v>
       </c>
       <c r="C202" s="20" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D202" s="22"/>
       <c r="E202" s="22" t="s">
@@ -11012,13 +11012,13 @@
     </row>
     <row r="203" spans="1:9">
       <c r="A203" s="22" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B203" s="30" t="s">
         <v>404</v>
       </c>
       <c r="C203" s="20" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D203" s="22"/>
       <c r="E203" s="22" t="s">
@@ -11037,13 +11037,13 @@
     </row>
     <row r="204" spans="1:9">
       <c r="A204" s="22" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B204" s="30" t="s">
         <v>404</v>
       </c>
       <c r="C204" s="20" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="D204" s="36"/>
       <c r="E204" s="22" t="s">
@@ -11537,13 +11537,13 @@
     </row>
     <row r="224" spans="1:9" ht="30">
       <c r="A224" s="22" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B224" s="30" t="s">
         <v>405</v>
       </c>
       <c r="C224" s="20" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D224" s="22"/>
       <c r="E224" s="22" t="s">
@@ -11562,13 +11562,13 @@
     </row>
     <row r="225" spans="1:9" ht="30">
       <c r="A225" s="22" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B225" s="30" t="s">
         <v>405</v>
       </c>
       <c r="C225" s="20" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D225" s="22"/>
       <c r="E225" s="22" t="s">
@@ -11587,13 +11587,13 @@
     </row>
     <row r="226" spans="1:9" ht="30">
       <c r="A226" s="22" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B226" s="30" t="s">
         <v>405</v>
       </c>
       <c r="C226" s="20" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D226" s="22"/>
       <c r="E226" s="22" t="s">
@@ -11612,13 +11612,13 @@
     </row>
     <row r="227" spans="1:9" ht="30">
       <c r="A227" s="22" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B227" s="30" t="s">
         <v>405</v>
       </c>
       <c r="C227" s="20" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D227" s="22"/>
       <c r="E227" s="22" t="s">
@@ -11637,13 +11637,13 @@
     </row>
     <row r="228" spans="1:9" ht="30">
       <c r="A228" s="22" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B228" s="30" t="s">
         <v>405</v>
       </c>
       <c r="C228" s="20" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="D228" s="36"/>
       <c r="E228" s="22" t="s">
@@ -11668,7 +11668,7 @@
         <v>406</v>
       </c>
       <c r="C229" s="20" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="D229" s="29"/>
       <c r="E229" s="29" t="s">
@@ -11768,7 +11768,7 @@
         <v>406</v>
       </c>
       <c r="C233" s="20" t="s">
-        <v>531</v>
+        <v>1055</v>
       </c>
       <c r="D233" s="29"/>
       <c r="E233" s="29" t="s">
@@ -11793,7 +11793,7 @@
         <v>406</v>
       </c>
       <c r="C234" s="31" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D234" s="29"/>
       <c r="E234" s="29" t="s">
@@ -11818,7 +11818,7 @@
         <v>406</v>
       </c>
       <c r="C235" s="31" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D235" s="29"/>
       <c r="E235" s="29" t="s">
@@ -11843,7 +11843,7 @@
         <v>406</v>
       </c>
       <c r="C236" s="31" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D236" s="29"/>
       <c r="E236" s="29" t="s">
@@ -11868,7 +11868,7 @@
         <v>406</v>
       </c>
       <c r="C237" s="20" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D237" s="29"/>
       <c r="E237" s="29" t="s">
@@ -11887,13 +11887,13 @@
     </row>
     <row r="238" spans="1:9" ht="30">
       <c r="A238" s="22" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B238" s="30" t="s">
         <v>406</v>
       </c>
       <c r="C238" s="20" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D238" s="22"/>
       <c r="E238" s="22" t="s">
@@ -11912,13 +11912,13 @@
     </row>
     <row r="239" spans="1:9" ht="30">
       <c r="A239" s="22" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B239" s="30" t="s">
         <v>406</v>
       </c>
       <c r="C239" s="20" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D239" s="22"/>
       <c r="E239" s="22" t="s">
@@ -11937,13 +11937,13 @@
     </row>
     <row r="240" spans="1:9" ht="30">
       <c r="A240" s="22" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B240" s="30" t="s">
         <v>406</v>
       </c>
       <c r="C240" s="20" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D240" s="22"/>
       <c r="E240" s="22" t="s">
@@ -11962,13 +11962,13 @@
     </row>
     <row r="241" spans="1:9" ht="30">
       <c r="A241" s="22" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B241" s="30" t="s">
         <v>406</v>
       </c>
       <c r="C241" s="20" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D241" s="22"/>
       <c r="E241" s="22" t="s">
@@ -11987,13 +11987,13 @@
     </row>
     <row r="242" spans="1:9" ht="30">
       <c r="A242" s="22" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B242" s="30" t="s">
         <v>406</v>
       </c>
       <c r="C242" s="20" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="D242" s="36"/>
       <c r="E242" s="22" t="s">
@@ -12018,7 +12018,7 @@
         <v>407</v>
       </c>
       <c r="C243" s="31" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D243" s="29"/>
       <c r="E243" s="29" t="s">
@@ -12043,7 +12043,7 @@
         <v>407</v>
       </c>
       <c r="C244" s="31" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D244" s="29"/>
       <c r="E244" s="29" t="s">
@@ -12068,7 +12068,7 @@
         <v>407</v>
       </c>
       <c r="C245" s="31" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D245" s="29"/>
       <c r="E245" s="29" t="s">
@@ -12093,7 +12093,7 @@
         <v>407</v>
       </c>
       <c r="C246" s="31" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D246" s="29"/>
       <c r="E246" s="29" t="s">
@@ -12118,7 +12118,7 @@
         <v>407</v>
       </c>
       <c r="C247" s="31" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D247" s="29"/>
       <c r="E247" s="29" t="s">
@@ -12143,7 +12143,7 @@
         <v>407</v>
       </c>
       <c r="C248" s="31" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D248" s="29"/>
       <c r="E248" s="29" t="s">
@@ -12168,7 +12168,7 @@
         <v>407</v>
       </c>
       <c r="C249" s="20" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D249" s="29"/>
       <c r="E249" s="29" t="s">
@@ -12187,13 +12187,13 @@
     </row>
     <row r="250" spans="1:9" ht="30">
       <c r="A250" s="22" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B250" s="30" t="s">
         <v>407</v>
       </c>
       <c r="C250" s="20" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D250" s="22"/>
       <c r="E250" s="22" t="s">
@@ -12212,13 +12212,13 @@
     </row>
     <row r="251" spans="1:9" ht="30">
       <c r="A251" s="22" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B251" s="30" t="s">
         <v>407</v>
       </c>
       <c r="C251" s="20" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D251" s="22"/>
       <c r="E251" s="22" t="s">
@@ -12237,13 +12237,13 @@
     </row>
     <row r="252" spans="1:9" ht="30">
       <c r="A252" s="22" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B252" s="30" t="s">
         <v>407</v>
       </c>
       <c r="C252" s="20" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D252" s="22"/>
       <c r="E252" s="22" t="s">
@@ -12262,13 +12262,13 @@
     </row>
     <row r="253" spans="1:9" ht="30">
       <c r="A253" s="22" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B253" s="30" t="s">
         <v>407</v>
       </c>
       <c r="C253" s="20" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D253" s="22"/>
       <c r="E253" s="22" t="s">
@@ -12287,13 +12287,13 @@
     </row>
     <row r="254" spans="1:9" ht="30">
       <c r="A254" s="22" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B254" s="30" t="s">
         <v>407</v>
       </c>
       <c r="C254" s="20" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="D254" s="36"/>
       <c r="E254" s="22" t="s">
@@ -12318,7 +12318,7 @@
         <v>408</v>
       </c>
       <c r="C255" s="20" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D255" s="29"/>
       <c r="E255" s="29" t="s">
@@ -12343,7 +12343,7 @@
         <v>408</v>
       </c>
       <c r="C256" s="31" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D256" s="29"/>
       <c r="E256" s="29" t="s">
@@ -12368,7 +12368,7 @@
         <v>408</v>
       </c>
       <c r="C257" s="31" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D257" s="29"/>
       <c r="E257" s="29" t="s">
@@ -12393,7 +12393,7 @@
         <v>408</v>
       </c>
       <c r="C258" s="31" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D258" s="29"/>
       <c r="E258" s="29" t="s">
@@ -12418,7 +12418,7 @@
         <v>408</v>
       </c>
       <c r="C259" s="31" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D259" s="29"/>
       <c r="E259" s="29" t="s">
@@ -12434,7 +12434,7 @@
         <v>17</v>
       </c>
       <c r="I259" s="31" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="260" spans="1:9" ht="30">
@@ -12445,10 +12445,10 @@
         <v>408</v>
       </c>
       <c r="C260" s="20" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D260" s="29" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E260" s="29" t="s">
         <v>19</v>
@@ -12466,13 +12466,13 @@
     </row>
     <row r="261" spans="1:9" ht="30">
       <c r="A261" s="22" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B261" s="30" t="s">
         <v>408</v>
       </c>
       <c r="C261" s="20" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D261" s="22"/>
       <c r="E261" s="22" t="s">
@@ -12491,13 +12491,13 @@
     </row>
     <row r="262" spans="1:9" ht="30">
       <c r="A262" s="22" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B262" s="30" t="s">
         <v>408</v>
       </c>
       <c r="C262" s="20" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D262" s="22"/>
       <c r="E262" s="22" t="s">
@@ -12516,13 +12516,13 @@
     </row>
     <row r="263" spans="1:9" ht="30">
       <c r="A263" s="22" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B263" s="30" t="s">
         <v>408</v>
       </c>
       <c r="C263" s="20" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D263" s="22"/>
       <c r="E263" s="22" t="s">
@@ -12541,13 +12541,13 @@
     </row>
     <row r="264" spans="1:9" ht="30">
       <c r="A264" s="22" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B264" s="30" t="s">
         <v>408</v>
       </c>
       <c r="C264" s="20" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D264" s="22"/>
       <c r="E264" s="22" t="s">
@@ -12566,13 +12566,13 @@
     </row>
     <row r="265" spans="1:9" ht="30">
       <c r="A265" s="22" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B265" s="30" t="s">
         <v>408</v>
       </c>
       <c r="C265" s="20" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="D265" s="36"/>
       <c r="E265" s="22" t="s">
@@ -12597,7 +12597,7 @@
         <v>409</v>
       </c>
       <c r="C266" s="20" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D266" s="29"/>
       <c r="E266" s="29" t="s">
@@ -12622,7 +12622,7 @@
         <v>409</v>
       </c>
       <c r="C267" s="20" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D267" s="29"/>
       <c r="E267" s="29" t="s">
@@ -12641,13 +12641,13 @@
     </row>
     <row r="268" spans="1:9">
       <c r="A268" s="22" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B268" s="30" t="s">
         <v>409</v>
       </c>
       <c r="C268" s="20" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="D268" s="36"/>
       <c r="E268" s="29" t="s">
@@ -12672,7 +12672,7 @@
         <v>410</v>
       </c>
       <c r="C269" s="31" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D269" s="29"/>
       <c r="E269" s="29" t="s">
@@ -12697,7 +12697,7 @@
         <v>410</v>
       </c>
       <c r="C270" s="31" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D270" s="29"/>
       <c r="E270" s="29" t="s">
@@ -12722,7 +12722,7 @@
         <v>410</v>
       </c>
       <c r="C271" s="31" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D271" s="29"/>
       <c r="E271" s="29" t="s">
@@ -12747,7 +12747,7 @@
         <v>410</v>
       </c>
       <c r="C272" s="31" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D272" s="29"/>
       <c r="E272" s="29" t="s">
@@ -12772,7 +12772,7 @@
         <v>410</v>
       </c>
       <c r="C273" s="31" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D273" s="29"/>
       <c r="E273" s="29" t="s">
@@ -12788,7 +12788,7 @@
         <v>17</v>
       </c>
       <c r="I273" s="31" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="274" spans="1:9" ht="30">
@@ -12799,10 +12799,10 @@
         <v>410</v>
       </c>
       <c r="C274" s="20" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D274" s="29" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E274" s="29" t="s">
         <v>19</v>
@@ -12820,13 +12820,13 @@
     </row>
     <row r="275" spans="1:9" ht="30">
       <c r="A275" s="22" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B275" s="30" t="s">
         <v>410</v>
       </c>
       <c r="C275" s="20" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D275" s="22"/>
       <c r="E275" s="22" t="s">
@@ -12845,13 +12845,13 @@
     </row>
     <row r="276" spans="1:9" ht="30">
       <c r="A276" s="22" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B276" s="30" t="s">
         <v>410</v>
       </c>
       <c r="C276" s="20" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D276" s="22"/>
       <c r="E276" s="22" t="s">
@@ -12870,13 +12870,13 @@
     </row>
     <row r="277" spans="1:9" ht="30">
       <c r="A277" s="22" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B277" s="30" t="s">
         <v>410</v>
       </c>
       <c r="C277" s="20" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D277" s="22"/>
       <c r="E277" s="22" t="s">
@@ -12895,13 +12895,13 @@
     </row>
     <row r="278" spans="1:9" ht="30">
       <c r="A278" s="22" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B278" s="30" t="s">
         <v>410</v>
       </c>
       <c r="C278" s="20" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D278" s="22"/>
       <c r="E278" s="22" t="s">
@@ -12920,13 +12920,13 @@
     </row>
     <row r="279" spans="1:9" ht="30">
       <c r="A279" s="22" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B279" s="30" t="s">
         <v>410</v>
       </c>
       <c r="C279" s="20" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="D279" s="36"/>
       <c r="E279" s="22" t="s">
@@ -12951,7 +12951,7 @@
         <v>411</v>
       </c>
       <c r="C280" s="31" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D280" s="29"/>
       <c r="E280" s="29" t="s">
@@ -12976,7 +12976,7 @@
         <v>411</v>
       </c>
       <c r="C281" s="31" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D281" s="29"/>
       <c r="E281" s="29" t="s">
@@ -13001,7 +13001,7 @@
         <v>411</v>
       </c>
       <c r="C282" s="31" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D282" s="29"/>
       <c r="E282" s="29" t="s">
@@ -13026,7 +13026,7 @@
         <v>411</v>
       </c>
       <c r="C283" s="31" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D283" s="29"/>
       <c r="E283" s="29" t="s">
@@ -13051,7 +13051,7 @@
         <v>411</v>
       </c>
       <c r="C284" s="31" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D284" s="29"/>
       <c r="E284" s="29" t="s">
@@ -13067,7 +13067,7 @@
         <v>17</v>
       </c>
       <c r="I284" s="31" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="285" spans="1:9" ht="30">
@@ -13078,10 +13078,10 @@
         <v>411</v>
       </c>
       <c r="C285" s="20" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D285" s="29" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E285" s="29" t="s">
         <v>19</v>
@@ -13099,13 +13099,13 @@
     </row>
     <row r="286" spans="1:9" ht="30">
       <c r="A286" s="22" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B286" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C286" s="20" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D286" s="22"/>
       <c r="E286" s="22" t="s">
@@ -13124,13 +13124,13 @@
     </row>
     <row r="287" spans="1:9" ht="30">
       <c r="A287" s="22" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B287" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C287" s="20" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D287" s="22"/>
       <c r="E287" s="22" t="s">
@@ -13149,13 +13149,13 @@
     </row>
     <row r="288" spans="1:9" ht="30">
       <c r="A288" s="22" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B288" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C288" s="20" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D288" s="22"/>
       <c r="E288" s="22" t="s">
@@ -13174,13 +13174,13 @@
     </row>
     <row r="289" spans="1:9" ht="30">
       <c r="A289" s="22" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B289" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C289" s="20" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D289" s="22"/>
       <c r="E289" s="22" t="s">
@@ -13199,13 +13199,13 @@
     </row>
     <row r="290" spans="1:9" ht="30">
       <c r="A290" s="22" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B290" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C290" s="20" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D290" s="36"/>
       <c r="E290" s="22" t="s">
@@ -13230,7 +13230,7 @@
         <v>412</v>
       </c>
       <c r="C291" s="20" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D291" s="29"/>
       <c r="E291" s="29" t="s">
@@ -13255,7 +13255,7 @@
         <v>412</v>
       </c>
       <c r="C292" s="20" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="D292" s="29"/>
       <c r="E292" s="29" t="s">
@@ -13280,7 +13280,7 @@
         <v>412</v>
       </c>
       <c r="C293" s="20" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="D293" s="29"/>
       <c r="E293" s="29" t="s">
@@ -13305,7 +13305,7 @@
         <v>412</v>
       </c>
       <c r="C294" s="31" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D294" s="29"/>
       <c r="E294" s="29" t="s">
@@ -13330,7 +13330,7 @@
         <v>412</v>
       </c>
       <c r="C295" s="31" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D295" s="29"/>
       <c r="E295" s="29" t="s">
@@ -13355,7 +13355,7 @@
         <v>412</v>
       </c>
       <c r="C296" s="20" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="D296" s="29"/>
       <c r="E296" s="29" t="s">
@@ -13374,13 +13374,13 @@
     </row>
     <row r="297" spans="1:9">
       <c r="A297" s="22" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B297" s="30" t="s">
         <v>412</v>
       </c>
       <c r="C297" s="20" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="D297" s="36"/>
       <c r="E297" s="29" t="s">
@@ -13405,7 +13405,7 @@
         <v>413</v>
       </c>
       <c r="C298" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D298" s="29"/>
       <c r="E298" s="29" t="s">
@@ -13430,7 +13430,7 @@
         <v>413</v>
       </c>
       <c r="C299" s="31" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D299" s="29"/>
       <c r="E299" s="29" t="s">
@@ -13455,7 +13455,7 @@
         <v>413</v>
       </c>
       <c r="C300" s="31" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D300" s="29"/>
       <c r="E300" s="29" t="s">
@@ -13474,13 +13474,13 @@
     </row>
     <row r="301" spans="1:9" ht="30">
       <c r="A301" s="22" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B301" s="30" t="s">
         <v>413</v>
       </c>
       <c r="C301" s="20" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D301" s="22"/>
       <c r="E301" s="22" t="s">
@@ -13499,13 +13499,13 @@
     </row>
     <row r="302" spans="1:9" ht="30">
       <c r="A302" s="22" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B302" s="30" t="s">
         <v>413</v>
       </c>
       <c r="C302" s="20" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D302" s="22"/>
       <c r="E302" s="22" t="s">
@@ -13524,13 +13524,13 @@
     </row>
     <row r="303" spans="1:9" ht="30">
       <c r="A303" s="22" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B303" s="30" t="s">
         <v>413</v>
       </c>
       <c r="C303" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D303" s="22"/>
       <c r="E303" s="22" t="s">
@@ -13549,13 +13549,13 @@
     </row>
     <row r="304" spans="1:9" ht="30">
       <c r="A304" s="22" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B304" s="30" t="s">
         <v>413</v>
       </c>
       <c r="C304" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D304" s="22"/>
       <c r="E304" s="22" t="s">
@@ -13574,13 +13574,13 @@
     </row>
     <row r="305" spans="1:9" ht="30">
       <c r="A305" s="22" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B305" s="30" t="s">
         <v>413</v>
       </c>
       <c r="C305" s="20" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D305" s="36"/>
       <c r="E305" s="22" t="s">
@@ -13605,7 +13605,7 @@
         <v>414</v>
       </c>
       <c r="C306" s="31" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D306" s="29"/>
       <c r="E306" s="29" t="s">
@@ -13630,7 +13630,7 @@
         <v>414</v>
       </c>
       <c r="C307" s="31" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D307" s="29"/>
       <c r="E307" s="29" t="s">
@@ -13655,7 +13655,7 @@
         <v>414</v>
       </c>
       <c r="C308" s="20" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D308" s="29"/>
       <c r="E308" s="29" t="s">
@@ -13674,13 +13674,13 @@
     </row>
     <row r="309" spans="1:9" ht="30">
       <c r="A309" s="22" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B309" s="30" t="s">
         <v>414</v>
       </c>
       <c r="C309" s="20" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D309" s="22"/>
       <c r="E309" s="22" t="s">
@@ -13699,13 +13699,13 @@
     </row>
     <row r="310" spans="1:9" ht="30">
       <c r="A310" s="22" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B310" s="30" t="s">
         <v>414</v>
       </c>
       <c r="C310" s="20" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D310" s="22"/>
       <c r="E310" s="22" t="s">
@@ -13724,13 +13724,13 @@
     </row>
     <row r="311" spans="1:9" ht="30">
       <c r="A311" s="22" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B311" s="30" t="s">
         <v>414</v>
       </c>
       <c r="C311" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D311" s="22"/>
       <c r="E311" s="22" t="s">
@@ -13749,13 +13749,13 @@
     </row>
     <row r="312" spans="1:9" ht="30">
       <c r="A312" s="22" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B312" s="30" t="s">
         <v>414</v>
       </c>
       <c r="C312" s="20" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D312" s="22"/>
       <c r="E312" s="22" t="s">
@@ -13774,13 +13774,13 @@
     </row>
     <row r="313" spans="1:9" ht="30">
       <c r="A313" s="22" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B313" s="30" t="s">
         <v>414</v>
       </c>
       <c r="C313" s="20" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D313" s="36"/>
       <c r="E313" s="22" t="s">
@@ -13805,7 +13805,7 @@
         <v>415</v>
       </c>
       <c r="C314" s="20" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D314" s="29"/>
       <c r="E314" s="29" t="s">
@@ -13830,7 +13830,7 @@
         <v>415</v>
       </c>
       <c r="C315" s="31" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D315" s="29"/>
       <c r="E315" s="29" t="s">
@@ -13855,7 +13855,7 @@
         <v>415</v>
       </c>
       <c r="C316" s="31" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D316" s="29"/>
       <c r="E316" s="29" t="s">
@@ -13880,7 +13880,7 @@
         <v>415</v>
       </c>
       <c r="C317" s="31" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D317" s="29"/>
       <c r="E317" s="29" t="s">
@@ -13905,7 +13905,7 @@
         <v>415</v>
       </c>
       <c r="C318" s="31" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D318" s="29"/>
       <c r="E318" s="29" t="s">
@@ -13930,7 +13930,7 @@
         <v>415</v>
       </c>
       <c r="C319" s="31" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D319" s="29"/>
       <c r="E319" s="29" t="s">
@@ -13949,13 +13949,13 @@
     </row>
     <row r="320" spans="1:9" ht="30">
       <c r="A320" s="22" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B320" s="30" t="s">
         <v>415</v>
       </c>
       <c r="C320" s="20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D320" s="22"/>
       <c r="E320" s="22" t="s">
@@ -13974,13 +13974,13 @@
     </row>
     <row r="321" spans="1:9" ht="30">
       <c r="A321" s="22" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B321" s="30" t="s">
         <v>415</v>
       </c>
       <c r="C321" s="20" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D321" s="22"/>
       <c r="E321" s="22" t="s">
@@ -13999,13 +13999,13 @@
     </row>
     <row r="322" spans="1:9" ht="30">
       <c r="A322" s="22" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B322" s="30" t="s">
         <v>415</v>
       </c>
       <c r="C322" s="20" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D322" s="22"/>
       <c r="E322" s="22" t="s">
@@ -14024,13 +14024,13 @@
     </row>
     <row r="323" spans="1:9" ht="30">
       <c r="A323" s="22" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B323" s="30" t="s">
         <v>415</v>
       </c>
       <c r="C323" s="20" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D323" s="22"/>
       <c r="E323" s="22" t="s">
@@ -14049,13 +14049,13 @@
     </row>
     <row r="324" spans="1:9" ht="30">
       <c r="A324" s="22" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B324" s="30" t="s">
         <v>415</v>
       </c>
       <c r="C324" s="20" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D324" s="36"/>
       <c r="E324" s="22" t="s">
@@ -14080,7 +14080,7 @@
         <v>416</v>
       </c>
       <c r="C325" s="31" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D325" s="29"/>
       <c r="E325" s="29" t="s">
@@ -14105,7 +14105,7 @@
         <v>416</v>
       </c>
       <c r="C326" s="20" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D326" s="29"/>
       <c r="E326" s="29" t="s">
@@ -14124,13 +14124,13 @@
     </row>
     <row r="327" spans="1:9">
       <c r="A327" s="22" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B327" s="30" t="s">
         <v>416</v>
       </c>
       <c r="C327" s="20" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D327" s="36"/>
       <c r="E327" s="29" t="s">
@@ -14155,7 +14155,7 @@
         <v>417</v>
       </c>
       <c r="C328" s="31" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D328" s="29"/>
       <c r="E328" s="29" t="s">
@@ -14180,7 +14180,7 @@
         <v>417</v>
       </c>
       <c r="C329" s="31" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D329" s="29"/>
       <c r="E329" s="29" t="s">
@@ -14205,7 +14205,7 @@
         <v>417</v>
       </c>
       <c r="C330" s="31" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D330" s="29"/>
       <c r="E330" s="29" t="s">
@@ -14230,7 +14230,7 @@
         <v>417</v>
       </c>
       <c r="C331" s="31" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D331" s="29"/>
       <c r="E331" s="29" t="s">
@@ -14255,7 +14255,7 @@
         <v>417</v>
       </c>
       <c r="C332" s="31" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D332" s="29"/>
       <c r="E332" s="29" t="s">
@@ -14271,7 +14271,7 @@
         <v>17</v>
       </c>
       <c r="I332" s="31" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="333" spans="1:9" ht="30">
@@ -14282,10 +14282,10 @@
         <v>417</v>
       </c>
       <c r="C333" s="20" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D333" s="29" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E333" s="29" t="s">
         <v>19</v>
@@ -14303,13 +14303,13 @@
     </row>
     <row r="334" spans="1:9" ht="30">
       <c r="A334" s="22" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B334" s="30" t="s">
         <v>417</v>
       </c>
       <c r="C334" s="20" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D334" s="22"/>
       <c r="E334" s="22" t="s">
@@ -14328,13 +14328,13 @@
     </row>
     <row r="335" spans="1:9" ht="30">
       <c r="A335" s="22" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B335" s="30" t="s">
         <v>417</v>
       </c>
       <c r="C335" s="20" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D335" s="22"/>
       <c r="E335" s="22" t="s">
@@ -14353,13 +14353,13 @@
     </row>
     <row r="336" spans="1:9" ht="30">
       <c r="A336" s="22" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B336" s="30" t="s">
         <v>417</v>
       </c>
       <c r="C336" s="20" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D336" s="22"/>
       <c r="E336" s="22" t="s">
@@ -14378,13 +14378,13 @@
     </row>
     <row r="337" spans="1:9" ht="30">
       <c r="A337" s="22" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B337" s="30" t="s">
         <v>417</v>
       </c>
       <c r="C337" s="20" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D337" s="22"/>
       <c r="E337" s="22" t="s">
@@ -14403,13 +14403,13 @@
     </row>
     <row r="338" spans="1:9" ht="30">
       <c r="A338" s="22" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B338" s="30" t="s">
         <v>417</v>
       </c>
       <c r="C338" s="20" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D338" s="36"/>
       <c r="E338" s="22" t="s">
@@ -14434,7 +14434,7 @@
         <v>418</v>
       </c>
       <c r="C339" s="31" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D339" s="29"/>
       <c r="E339" s="29" t="s">
@@ -14459,7 +14459,7 @@
         <v>418</v>
       </c>
       <c r="C340" s="31" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D340" s="29"/>
       <c r="E340" s="29" t="s">
@@ -14484,7 +14484,7 @@
         <v>418</v>
       </c>
       <c r="C341" s="31" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D341" s="29"/>
       <c r="E341" s="29" t="s">
@@ -14509,7 +14509,7 @@
         <v>418</v>
       </c>
       <c r="C342" s="31" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D342" s="29"/>
       <c r="E342" s="29" t="s">
@@ -14534,7 +14534,7 @@
         <v>418</v>
       </c>
       <c r="C343" s="31" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D343" s="29"/>
       <c r="E343" s="29" t="s">
@@ -14550,7 +14550,7 @@
         <v>17</v>
       </c>
       <c r="I343" s="31" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="344" spans="1:9" ht="30">
@@ -14561,10 +14561,10 @@
         <v>418</v>
       </c>
       <c r="C344" s="20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D344" s="29" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E344" s="29" t="s">
         <v>19</v>
@@ -14582,13 +14582,13 @@
     </row>
     <row r="345" spans="1:9" ht="30">
       <c r="A345" s="22" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B345" s="30" t="s">
         <v>418</v>
       </c>
       <c r="C345" s="20" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D345" s="22"/>
       <c r="E345" s="22" t="s">
@@ -14607,13 +14607,13 @@
     </row>
     <row r="346" spans="1:9" ht="30">
       <c r="A346" s="22" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B346" s="30" t="s">
         <v>418</v>
       </c>
       <c r="C346" s="20" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D346" s="22"/>
       <c r="E346" s="22" t="s">
@@ -14632,13 +14632,13 @@
     </row>
     <row r="347" spans="1:9" ht="30">
       <c r="A347" s="22" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B347" s="30" t="s">
         <v>418</v>
       </c>
       <c r="C347" s="20" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D347" s="22"/>
       <c r="E347" s="22" t="s">
@@ -14657,13 +14657,13 @@
     </row>
     <row r="348" spans="1:9" ht="30">
       <c r="A348" s="22" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B348" s="30" t="s">
         <v>418</v>
       </c>
       <c r="C348" s="20" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D348" s="22"/>
       <c r="E348" s="22" t="s">
@@ -14682,13 +14682,13 @@
     </row>
     <row r="349" spans="1:9" ht="30">
       <c r="A349" s="22" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B349" s="30" t="s">
         <v>418</v>
       </c>
       <c r="C349" s="20" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D349" s="36"/>
       <c r="E349" s="22" t="s">
@@ -14713,7 +14713,7 @@
         <v>419</v>
       </c>
       <c r="C350" s="31" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D350" s="29"/>
       <c r="E350" s="29" t="s">
@@ -14738,7 +14738,7 @@
         <v>31</v>
       </c>
       <c r="C351" s="20" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D351" s="29"/>
       <c r="E351" s="29" t="s">
@@ -14763,7 +14763,7 @@
         <v>31</v>
       </c>
       <c r="C352" s="31" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D352" s="29"/>
       <c r="E352" s="29" t="s">
@@ -14788,7 +14788,7 @@
         <v>31</v>
       </c>
       <c r="C353" s="31" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D353" s="29"/>
       <c r="E353" s="29" t="s">
@@ -14813,7 +14813,7 @@
         <v>31</v>
       </c>
       <c r="C354" s="20" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D354" s="29"/>
       <c r="E354" s="29" t="s">
@@ -14838,7 +14838,7 @@
         <v>31</v>
       </c>
       <c r="C355" s="20" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D355" s="29"/>
       <c r="E355" s="29" t="s">
@@ -14863,7 +14863,7 @@
         <v>31</v>
       </c>
       <c r="C356" s="20" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D356" s="29"/>
       <c r="E356" s="29" t="s">
@@ -14888,7 +14888,7 @@
         <v>32</v>
       </c>
       <c r="C357" s="20" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D357" s="29"/>
       <c r="E357" s="29" t="s">
@@ -14913,7 +14913,7 @@
         <v>32</v>
       </c>
       <c r="C358" s="31" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D358" s="29"/>
       <c r="E358" s="29" t="s">
@@ -14938,7 +14938,7 @@
         <v>32</v>
       </c>
       <c r="C359" s="20" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D359" s="29"/>
       <c r="E359" s="29" t="s">
@@ -14963,7 +14963,7 @@
         <v>32</v>
       </c>
       <c r="C360" s="31" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D360" s="29"/>
       <c r="E360" s="29" t="s">
@@ -14988,7 +14988,7 @@
         <v>420</v>
       </c>
       <c r="C361" s="20" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D361" s="29"/>
       <c r="E361" s="29" t="s">
@@ -15013,7 +15013,7 @@
         <v>420</v>
       </c>
       <c r="C362" s="31" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D362" s="29"/>
       <c r="E362" s="29" t="s">
@@ -15038,7 +15038,7 @@
         <v>421</v>
       </c>
       <c r="C363" s="20" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D363" s="29"/>
       <c r="E363" s="29" t="s">
@@ -15063,7 +15063,7 @@
         <v>422</v>
       </c>
       <c r="C364" s="31" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D364" s="29"/>
       <c r="E364" s="29" t="s">
@@ -15088,7 +15088,7 @@
         <v>423</v>
       </c>
       <c r="C365" s="20" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D365" s="29"/>
       <c r="E365" s="29" t="s">
@@ -15113,7 +15113,7 @@
         <v>423</v>
       </c>
       <c r="C366" s="31" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D366" s="29"/>
       <c r="E366" s="29" t="s">
@@ -15138,7 +15138,7 @@
         <v>423</v>
       </c>
       <c r="C367" s="31" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D367" s="29"/>
       <c r="E367" s="29" t="s">
@@ -15163,7 +15163,7 @@
         <v>423</v>
       </c>
       <c r="C368" s="31" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D368" s="29"/>
       <c r="E368" s="29" t="s">
@@ -15188,7 +15188,7 @@
         <v>423</v>
       </c>
       <c r="C369" s="31" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D369" s="29"/>
       <c r="E369" s="29" t="s">
@@ -15213,7 +15213,7 @@
         <v>423</v>
       </c>
       <c r="C370" s="31" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D370" s="29"/>
       <c r="E370" s="29" t="s">
@@ -15238,7 +15238,7 @@
         <v>423</v>
       </c>
       <c r="C371" s="31" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D371" s="29"/>
       <c r="E371" s="29" t="s">
@@ -15263,7 +15263,7 @@
         <v>423</v>
       </c>
       <c r="C372" s="31" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D372" s="29"/>
       <c r="E372" s="29" t="s">
@@ -15288,7 +15288,7 @@
         <v>423</v>
       </c>
       <c r="C373" s="31" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D373" s="29"/>
       <c r="E373" s="29" t="s">
@@ -15313,7 +15313,7 @@
         <v>424</v>
       </c>
       <c r="C374" s="31" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D374" s="29"/>
       <c r="E374" s="29" t="s">
@@ -15338,7 +15338,7 @@
         <v>424</v>
       </c>
       <c r="C375" s="31" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D375" s="29"/>
       <c r="E375" s="29" t="s">
@@ -15363,7 +15363,7 @@
         <v>424</v>
       </c>
       <c r="C376" s="31" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D376" s="29"/>
       <c r="E376" s="29" t="s">
@@ -15388,7 +15388,7 @@
         <v>424</v>
       </c>
       <c r="C377" s="31" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D377" s="29"/>
       <c r="E377" s="29" t="s">
@@ -15413,7 +15413,7 @@
         <v>424</v>
       </c>
       <c r="C378" s="31" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D378" s="29"/>
       <c r="E378" s="29" t="s">
@@ -15438,7 +15438,7 @@
         <v>424</v>
       </c>
       <c r="C379" s="31" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D379" s="29"/>
       <c r="E379" s="29" t="s">
@@ -15463,7 +15463,7 @@
         <v>424</v>
       </c>
       <c r="C380" s="31" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D380" s="29"/>
       <c r="E380" s="29" t="s">
@@ -15488,7 +15488,7 @@
         <v>424</v>
       </c>
       <c r="C381" s="31" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D381" s="29"/>
       <c r="E381" s="29" t="s">
@@ -15513,7 +15513,7 @@
         <v>424</v>
       </c>
       <c r="C382" s="31" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D382" s="29"/>
       <c r="E382" s="29" t="s">
@@ -15538,7 +15538,7 @@
         <v>424</v>
       </c>
       <c r="C383" s="31" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D383" s="29"/>
       <c r="E383" s="29" t="s">
@@ -15563,7 +15563,7 @@
         <v>424</v>
       </c>
       <c r="C384" s="31" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D384" s="29"/>
       <c r="E384" s="29" t="s">
@@ -15588,7 +15588,7 @@
         <v>425</v>
       </c>
       <c r="C385" s="31" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D385" s="29"/>
       <c r="E385" s="29" t="s">
@@ -15613,7 +15613,7 @@
         <v>425</v>
       </c>
       <c r="C386" s="31" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D386" s="29"/>
       <c r="E386" s="29" t="s">
@@ -15638,7 +15638,7 @@
         <v>425</v>
       </c>
       <c r="C387" s="31" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D387" s="29"/>
       <c r="E387" s="29" t="s">
@@ -15663,7 +15663,7 @@
         <v>425</v>
       </c>
       <c r="C388" s="31" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D388" s="29"/>
       <c r="E388" s="29" t="s">
@@ -15688,7 +15688,7 @@
         <v>425</v>
       </c>
       <c r="C389" s="20" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="D389" s="29"/>
       <c r="E389" s="29" t="s">
@@ -15713,7 +15713,7 @@
         <v>425</v>
       </c>
       <c r="C390" s="20" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D390" s="29"/>
       <c r="E390" s="29" t="s">
@@ -15738,7 +15738,7 @@
         <v>425</v>
       </c>
       <c r="C391" s="31" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D391" s="29"/>
       <c r="E391" s="29" t="s">
@@ -15763,7 +15763,7 @@
         <v>425</v>
       </c>
       <c r="C392" s="31" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D392" s="29"/>
       <c r="E392" s="29" t="s">
@@ -15788,7 +15788,7 @@
         <v>425</v>
       </c>
       <c r="C393" s="31" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D393" s="29"/>
       <c r="E393" s="29" t="s">
@@ -15813,7 +15813,7 @@
         <v>425</v>
       </c>
       <c r="C394" s="31" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D394" s="29"/>
       <c r="E394" s="29" t="s">
@@ -15838,7 +15838,7 @@
         <v>425</v>
       </c>
       <c r="C395" s="31" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D395" s="29"/>
       <c r="E395" s="29" t="s">
@@ -15863,7 +15863,7 @@
         <v>425</v>
       </c>
       <c r="C396" s="31" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D396" s="29"/>
       <c r="E396" s="29" t="s">
@@ -15888,7 +15888,7 @@
         <v>425</v>
       </c>
       <c r="C397" s="31" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D397" s="29"/>
       <c r="E397" s="29" t="s">
@@ -15913,7 +15913,7 @@
         <v>425</v>
       </c>
       <c r="C398" s="31" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D398" s="29"/>
       <c r="E398" s="29" t="s">
@@ -15938,7 +15938,7 @@
         <v>425</v>
       </c>
       <c r="C399" s="31" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D399" s="29"/>
       <c r="E399" s="29" t="s">
@@ -15963,7 +15963,7 @@
         <v>426</v>
       </c>
       <c r="C400" s="31" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D400" s="29"/>
       <c r="E400" s="29" t="s">
@@ -15988,7 +15988,7 @@
         <v>426</v>
       </c>
       <c r="C401" s="20" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D401" s="29"/>
       <c r="E401" s="29" t="s">
@@ -16004,18 +16004,18 @@
         <v>17</v>
       </c>
       <c r="I401" s="31" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="402" spans="1:9" ht="30">
       <c r="A402" s="22" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B402" s="30" t="s">
         <v>426</v>
       </c>
       <c r="C402" s="20" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D402" s="36"/>
       <c r="E402" s="29" t="s">
@@ -16040,7 +16040,7 @@
         <v>427</v>
       </c>
       <c r="C403" s="33" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D403" s="29"/>
       <c r="E403" s="29" t="s">
@@ -16065,7 +16065,7 @@
         <v>427</v>
       </c>
       <c r="C404" s="20" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D404" s="29"/>
       <c r="E404" s="29" t="s">
@@ -16090,7 +16090,7 @@
         <v>427</v>
       </c>
       <c r="C405" s="20" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D405" s="29"/>
       <c r="E405" s="29" t="s">
@@ -16115,7 +16115,7 @@
         <v>427</v>
       </c>
       <c r="C406" s="31" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D406" s="29"/>
       <c r="E406" s="29" t="s">
@@ -16140,7 +16140,7 @@
         <v>427</v>
       </c>
       <c r="C407" s="31" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D407" s="29"/>
       <c r="E407" s="29" t="s">
@@ -16165,7 +16165,7 @@
         <v>427</v>
       </c>
       <c r="C408" s="31" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D408" s="29"/>
       <c r="E408" s="29" t="s">
@@ -16190,7 +16190,7 @@
         <v>427</v>
       </c>
       <c r="C409" s="31" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D409" s="29"/>
       <c r="E409" s="29" t="s">
@@ -16215,7 +16215,7 @@
         <v>427</v>
       </c>
       <c r="C410" s="31" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D410" s="29"/>
       <c r="E410" s="29" t="s">
@@ -16240,7 +16240,7 @@
         <v>427</v>
       </c>
       <c r="C411" s="20" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D411" s="29"/>
       <c r="E411" s="29" t="s">
@@ -16265,7 +16265,7 @@
         <v>427</v>
       </c>
       <c r="C412" s="31" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D412" s="29"/>
       <c r="E412" s="29" t="s">
@@ -16290,7 +16290,7 @@
         <v>427</v>
       </c>
       <c r="C413" s="31" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D413" s="29"/>
       <c r="E413" s="29" t="s">
@@ -16315,7 +16315,7 @@
         <v>427</v>
       </c>
       <c r="C414" s="31" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D414" s="29"/>
       <c r="E414" s="29" t="s">
@@ -16340,7 +16340,7 @@
         <v>427</v>
       </c>
       <c r="C415" s="20" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D415" s="29"/>
       <c r="E415" s="29" t="s">
@@ -16365,7 +16365,7 @@
         <v>427</v>
       </c>
       <c r="C416" s="31" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D416" s="29"/>
       <c r="E416" s="29" t="s">
@@ -16390,7 +16390,7 @@
         <v>427</v>
       </c>
       <c r="C417" s="31" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D417" s="29"/>
       <c r="E417" s="29" t="s">
@@ -16415,7 +16415,7 @@
         <v>427</v>
       </c>
       <c r="C418" s="20" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D418" s="29"/>
       <c r="E418" s="29" t="s">
@@ -16440,7 +16440,7 @@
         <v>427</v>
       </c>
       <c r="C419" s="31" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D419" s="29"/>
       <c r="E419" s="29" t="s">
@@ -16465,7 +16465,7 @@
         <v>427</v>
       </c>
       <c r="C420" s="31" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D420" s="29"/>
       <c r="E420" s="29" t="s">
@@ -16490,7 +16490,7 @@
         <v>427</v>
       </c>
       <c r="C421" s="31" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D421" s="29"/>
       <c r="E421" s="29" t="s">
@@ -16515,7 +16515,7 @@
         <v>427</v>
       </c>
       <c r="C422" s="31" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D422" s="29"/>
       <c r="E422" s="29" t="s">
@@ -16540,7 +16540,7 @@
         <v>427</v>
       </c>
       <c r="C423" s="31" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D423" s="29"/>
       <c r="E423" s="29" t="s">
@@ -16565,7 +16565,7 @@
         <v>427</v>
       </c>
       <c r="C424" s="20" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="D424" s="29"/>
       <c r="E424" s="29" t="s">
@@ -16590,7 +16590,7 @@
         <v>427</v>
       </c>
       <c r="C425" s="31" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D425" s="29"/>
       <c r="E425" s="29" t="s">
@@ -16615,7 +16615,7 @@
         <v>427</v>
       </c>
       <c r="C426" s="31" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D426" s="29"/>
       <c r="E426" s="29" t="s">
@@ -16640,7 +16640,7 @@
         <v>427</v>
       </c>
       <c r="C427" s="31" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D427" s="29"/>
       <c r="E427" s="29" t="s">
@@ -16665,7 +16665,7 @@
         <v>427</v>
       </c>
       <c r="C428" s="20" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="D428" s="29"/>
       <c r="E428" s="29" t="s">
@@ -16690,7 +16690,7 @@
         <v>427</v>
       </c>
       <c r="C429" s="31" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D429" s="29"/>
       <c r="E429" s="29" t="s">
@@ -16715,7 +16715,7 @@
         <v>427</v>
       </c>
       <c r="C430" s="31" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D430" s="29"/>
       <c r="E430" s="29" t="s">
@@ -16740,7 +16740,7 @@
         <v>427</v>
       </c>
       <c r="C431" s="31" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D431" s="29"/>
       <c r="E431" s="29" t="s">
@@ -16765,7 +16765,7 @@
         <v>427</v>
       </c>
       <c r="C432" s="31" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D432" s="29"/>
       <c r="E432" s="29" t="s">
@@ -16790,7 +16790,7 @@
         <v>427</v>
       </c>
       <c r="C433" s="31" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D433" s="29"/>
       <c r="E433" s="29" t="s">
@@ -16815,7 +16815,7 @@
         <v>427</v>
       </c>
       <c r="C434" s="31" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D434" s="29"/>
       <c r="E434" s="29" t="s">
@@ -16840,7 +16840,7 @@
         <v>427</v>
       </c>
       <c r="C435" s="31" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D435" s="29"/>
       <c r="E435" s="29" t="s">
@@ -16865,7 +16865,7 @@
         <v>427</v>
       </c>
       <c r="C436" s="31" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D436" s="29"/>
       <c r="E436" s="29" t="s">
@@ -16890,7 +16890,7 @@
         <v>427</v>
       </c>
       <c r="C437" s="31" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D437" s="29"/>
       <c r="E437" s="29" t="s">
@@ -16915,7 +16915,7 @@
         <v>427</v>
       </c>
       <c r="C438" s="31" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D438" s="29"/>
       <c r="E438" s="29" t="s">
@@ -16940,7 +16940,7 @@
         <v>427</v>
       </c>
       <c r="C439" s="31" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D439" s="29"/>
       <c r="E439" s="29" t="s">
@@ -16965,7 +16965,7 @@
         <v>427</v>
       </c>
       <c r="C440" s="31" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D440" s="29"/>
       <c r="E440" s="29" t="s">
@@ -16990,7 +16990,7 @@
         <v>427</v>
       </c>
       <c r="C441" s="31" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D441" s="29"/>
       <c r="E441" s="29" t="s">
@@ -17015,7 +17015,7 @@
         <v>427</v>
       </c>
       <c r="C442" s="31" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D442" s="29"/>
       <c r="E442" s="29" t="s">
@@ -17040,7 +17040,7 @@
         <v>427</v>
       </c>
       <c r="C443" s="31" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D443" s="29"/>
       <c r="E443" s="29" t="s">
@@ -17065,7 +17065,7 @@
         <v>427</v>
       </c>
       <c r="C444" s="31" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D444" s="29"/>
       <c r="E444" s="29" t="s">
@@ -17090,7 +17090,7 @@
         <v>427</v>
       </c>
       <c r="C445" s="31" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D445" s="29"/>
       <c r="E445" s="29" t="s">
@@ -17115,7 +17115,7 @@
         <v>427</v>
       </c>
       <c r="C446" s="20" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D446" s="29"/>
       <c r="E446" s="29" t="s">
@@ -17140,7 +17140,7 @@
         <v>427</v>
       </c>
       <c r="C447" s="20" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D447" s="29"/>
       <c r="E447" s="29" t="s">
@@ -17165,7 +17165,7 @@
         <v>427</v>
       </c>
       <c r="C448" s="20" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D448" s="29"/>
       <c r="E448" s="29" t="s">
@@ -17190,7 +17190,7 @@
         <v>427</v>
       </c>
       <c r="C449" s="20" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D449" s="29"/>
       <c r="E449" s="29" t="s">
@@ -17215,7 +17215,7 @@
         <v>427</v>
       </c>
       <c r="C450" s="20" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D450" s="29"/>
       <c r="E450" s="29" t="s">
@@ -17240,7 +17240,7 @@
         <v>427</v>
       </c>
       <c r="C451" s="20" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D451" s="29"/>
       <c r="E451" s="29" t="s">
@@ -17265,7 +17265,7 @@
         <v>427</v>
       </c>
       <c r="C452" s="20" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D452" s="29"/>
       <c r="E452" s="29" t="s">
@@ -17290,7 +17290,7 @@
         <v>427</v>
       </c>
       <c r="C453" s="20" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D453" s="29"/>
       <c r="E453" s="29" t="s">
@@ -17315,7 +17315,7 @@
         <v>427</v>
       </c>
       <c r="C454" s="20" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D454" s="29"/>
       <c r="E454" s="29" t="s">
@@ -17340,7 +17340,7 @@
         <v>427</v>
       </c>
       <c r="C455" s="20" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D455" s="29"/>
       <c r="E455" s="29" t="s">
@@ -17365,7 +17365,7 @@
         <v>427</v>
       </c>
       <c r="C456" s="20" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D456" s="29"/>
       <c r="E456" s="29" t="s">
@@ -17390,7 +17390,7 @@
         <v>427</v>
       </c>
       <c r="C457" s="20" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D457" s="29"/>
       <c r="E457" s="29" t="s">
@@ -17415,7 +17415,7 @@
         <v>427</v>
       </c>
       <c r="C458" s="20" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D458" s="29"/>
       <c r="E458" s="29" t="s">
@@ -17440,7 +17440,7 @@
         <v>427</v>
       </c>
       <c r="C459" s="20" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D459" s="29"/>
       <c r="E459" s="29" t="s">
@@ -17465,7 +17465,7 @@
         <v>427</v>
       </c>
       <c r="C460" s="20" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D460" s="29"/>
       <c r="E460" s="29" t="s">
@@ -17490,7 +17490,7 @@
         <v>427</v>
       </c>
       <c r="C461" s="20" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D461" s="29"/>
       <c r="E461" s="29" t="s">
@@ -17515,7 +17515,7 @@
         <v>427</v>
       </c>
       <c r="C462" s="31" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D462" s="29"/>
       <c r="E462" s="29" t="s">
@@ -17540,7 +17540,7 @@
         <v>428</v>
       </c>
       <c r="C463" s="31" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D463" s="29"/>
       <c r="E463" s="29" t="s">
@@ -17565,7 +17565,7 @@
         <v>428</v>
       </c>
       <c r="C464" s="31" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D464" s="29"/>
       <c r="E464" s="29" t="s">
@@ -17590,10 +17590,10 @@
         <v>428</v>
       </c>
       <c r="C465" s="20" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D465" s="22" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E465" s="29" t="s">
         <v>22</v>
@@ -17608,7 +17608,7 @@
         <v>20</v>
       </c>
       <c r="I465" s="31" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="466" spans="1:9" ht="30">
@@ -17619,7 +17619,7 @@
         <v>429</v>
       </c>
       <c r="C466" s="20" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D466" s="29"/>
       <c r="E466" s="29" t="s">
@@ -17638,13 +17638,13 @@
     </row>
     <row r="467" spans="1:9" ht="30">
       <c r="A467" s="22" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B467" s="30" t="s">
         <v>430</v>
       </c>
       <c r="C467" s="20" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D467" s="36"/>
       <c r="E467" s="29" t="s">
@@ -17669,7 +17669,7 @@
         <v>430</v>
       </c>
       <c r="C468" s="20" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D468" s="29"/>
       <c r="E468" s="29" t="s">
@@ -17694,7 +17694,7 @@
         <v>430</v>
       </c>
       <c r="C469" s="20" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D469" s="29"/>
       <c r="E469" s="29" t="s">
@@ -17719,7 +17719,7 @@
         <v>430</v>
       </c>
       <c r="C470" s="20" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D470" s="29"/>
       <c r="E470" s="29" t="s">
@@ -17744,7 +17744,7 @@
         <v>430</v>
       </c>
       <c r="C471" s="20" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D471" s="29"/>
       <c r="E471" s="29" t="s">
@@ -17769,7 +17769,7 @@
         <v>430</v>
       </c>
       <c r="C472" s="20" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D472" s="29"/>
       <c r="E472" s="29" t="s">
@@ -17794,7 +17794,7 @@
         <v>430</v>
       </c>
       <c r="C473" s="20" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D473" s="29"/>
       <c r="E473" s="29" t="s">
@@ -17819,7 +17819,7 @@
         <v>430</v>
       </c>
       <c r="C474" s="20" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D474" s="29"/>
       <c r="E474" s="29" t="s">
@@ -17844,7 +17844,7 @@
         <v>430</v>
       </c>
       <c r="C475" s="20" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D475" s="29"/>
       <c r="E475" s="29" t="s">
@@ -17869,7 +17869,7 @@
         <v>430</v>
       </c>
       <c r="C476" s="20" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D476" s="29"/>
       <c r="E476" s="29" t="s">
@@ -17894,7 +17894,7 @@
         <v>430</v>
       </c>
       <c r="C477" s="20" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D477" s="29"/>
       <c r="E477" s="29" t="s">
@@ -17919,7 +17919,7 @@
         <v>430</v>
       </c>
       <c r="C478" s="20" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D478" s="29"/>
       <c r="E478" s="29" t="s">
@@ -17944,7 +17944,7 @@
         <v>430</v>
       </c>
       <c r="C479" s="20" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D479" s="29"/>
       <c r="E479" s="29" t="s">
@@ -17969,7 +17969,7 @@
         <v>430</v>
       </c>
       <c r="C480" s="20" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D480" s="29"/>
       <c r="E480" s="29" t="s">
@@ -17994,7 +17994,7 @@
         <v>430</v>
       </c>
       <c r="C481" s="20" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D481" s="29"/>
       <c r="E481" s="29" t="s">
@@ -18019,7 +18019,7 @@
         <v>430</v>
       </c>
       <c r="C482" s="20" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D482" s="29"/>
       <c r="E482" s="29" t="s">
@@ -18044,7 +18044,7 @@
         <v>430</v>
       </c>
       <c r="C483" s="20" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D483" s="29"/>
       <c r="E483" s="29" t="s">
@@ -18069,7 +18069,7 @@
         <v>430</v>
       </c>
       <c r="C484" s="20" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D484" s="29"/>
       <c r="E484" s="29" t="s">
@@ -18094,7 +18094,7 @@
         <v>430</v>
       </c>
       <c r="C485" s="20" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D485" s="29"/>
       <c r="E485" s="29" t="s">
@@ -18113,13 +18113,13 @@
     </row>
     <row r="486" spans="1:9" ht="30">
       <c r="A486" s="34" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B486" s="35" t="s">
         <v>430</v>
       </c>
       <c r="C486" s="20" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D486" s="22"/>
       <c r="E486" s="29" t="s">
@@ -18144,7 +18144,7 @@
         <v>389</v>
       </c>
       <c r="C487" s="20" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D487" s="29"/>
       <c r="E487" s="29" t="s">
@@ -18169,7 +18169,7 @@
         <v>389</v>
       </c>
       <c r="C488" s="31" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D488" s="29"/>
       <c r="E488" s="29" t="s">
@@ -18194,7 +18194,7 @@
         <v>389</v>
       </c>
       <c r="C489" s="31" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D489" s="29"/>
       <c r="E489" s="29" t="s">
@@ -18219,7 +18219,7 @@
         <v>390</v>
       </c>
       <c r="C490" s="31" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D490" s="29"/>
       <c r="E490" s="29" t="s">
@@ -18244,7 +18244,7 @@
         <v>390</v>
       </c>
       <c r="C491" s="31" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D491" s="29"/>
       <c r="E491" s="29" t="s">
@@ -18269,7 +18269,7 @@
         <v>431</v>
       </c>
       <c r="C492" s="31" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D492" s="29"/>
       <c r="E492" s="29" t="s">
@@ -18294,7 +18294,7 @@
         <v>431</v>
       </c>
       <c r="C493" s="31" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D493" s="29"/>
       <c r="E493" s="29" t="s">
@@ -18319,7 +18319,7 @@
         <v>431</v>
       </c>
       <c r="C494" s="31" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D494" s="29"/>
       <c r="E494" s="29" t="s">
@@ -18344,7 +18344,7 @@
         <v>431</v>
       </c>
       <c r="C495" s="31" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D495" s="29"/>
       <c r="E495" s="29" t="s">
@@ -18371,6 +18371,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -18378,11 +18383,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A403:B403 D403:I403 A468:B485 D468:I486 A20:H46 A34:I46 A101:I106 A112:I117 A135:I143 A149:I155 A173:I177 A183:I188 A194:I199 A205:I223 A229:I237 A243:I249 A255:I260 A280:I285 A306:I308 A314:I319 A339:I344 A65:I77 A83:I95 A161:I167 A47:B51 A96:B100 A78:B82 A60:B64 A52:I59 A118:B122 A107:B111 A130:B134 A144:B148 A156:B160 A168:B172 A178:B182 A189:B193 A200:B204 A224:B228 A238:B242 A250:B254 A261:B265 A266:I274 A275:B279 A286:B290 A291:I300 A301:B305 A309:B313 A320:B324 A325:I333 A334:B338 A345:B349 A350:I402 A487:I495 A404:I467 A123:I129 I20:I495">
@@ -19483,15 +19483,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -19540,6 +19531,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
@@ -19555,14 +19555,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19575,4 +19567,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>